<commit_message>
Fixed a results page bug and a entries page bug
Fixed some bugs
</commit_message>
<xml_diff>
--- a/static/downloads/single-crystal_db.xlsx
+++ b/static/downloads/single-crystal_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\Desktop\Mineral database website\static\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robbie\Documents\GitHub\Single-Crystal-Mineral-Database\static\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5CD5B2-C67F-4AEC-AD00-6CD9C6593779}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E401E842-4669-4014-A209-94E652173BC7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14388" windowHeight="3810" tabRatio="411" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6648" tabRatio="411" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cubic Minerals" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2254" uniqueCount="838">
   <si>
     <t>KBr</t>
   </si>
@@ -3584,9 +3584,6 @@
   </si>
   <si>
     <t>(Mn0.62Zn0.34)Fe2.04O4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Kim and Achenbach 92</t>
@@ -3885,7 +3882,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4041,6 +4038,9 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -4550,7 +4550,7 @@
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="AA232" sqref="AA232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="3" spans="1:37" ht="15">
       <c r="A3" s="63" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="4" spans="1:37" ht="15">
       <c r="A4" s="63" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -4623,7 +4623,7 @@
         <v>125</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>126</v>
@@ -31099,8 +31099,8 @@
         <f>SQRT((K231/N231) +4/3)</f>
         <v>1.6812637033649067</v>
       </c>
-      <c r="Y231" s="4" t="s">
-        <v>831</v>
+      <c r="Y231" s="64" t="s">
+        <v>169</v>
       </c>
       <c r="Z231" s="4">
         <f>I231/H231</f>
@@ -31990,6 +31990,9 @@
       <c r="F244" s="1">
         <v>1</v>
       </c>
+      <c r="G244" s="1" t="s">
+        <v>169</v>
+      </c>
       <c r="H244" s="33">
         <v>511</v>
       </c>
@@ -32041,11 +32044,11 @@
       </c>
       <c r="V244" s="6" t="e">
         <f>SQRT(K244/G244)</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="W244" s="6" t="e">
         <f>SQRT(N244/G244)</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="X244" s="4">
         <f>SQRT((K244/N244) +4/3)</f>
@@ -32386,12 +32389,12 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15">
       <c r="A1" s="63" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="63" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15">
@@ -36128,10 +36131,10 @@
         <v>174</v>
       </c>
       <c r="D238" s="22" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E238" s="40" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="239" spans="1:8">
@@ -36145,10 +36148,10 @@
         <v>174</v>
       </c>
       <c r="D239" s="22" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E239" s="40" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="240" spans="1:8">
@@ -36162,10 +36165,10 @@
         <v>174</v>
       </c>
       <c r="D240" s="22" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E240" s="40" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="242" spans="1:8">
@@ -36623,12 +36626,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15">
       <c r="A1" s="63" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15">
       <c r="A2" s="63" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -36826,7 +36829,7 @@
         <v>782</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.7">

</xml_diff>